<commit_message>
Update to Smartline_IUCNGET crosswalk
</commit_message>
<xml_diff>
--- a/crosswalks/Smartline-IUCNGET/Smartline-IUCNGET.xlsx
+++ b/crosswalks/Smartline-IUCNGET/Smartline-IUCNGET.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\Smartline-IUCNGET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/jor069_csiro_au/Documents/NEAP/ecosystem-typology/crosswalks/Smartline-IUCNGET/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48BD09D-4ADD-4A02-9010-043E4E867A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{B48BD09D-4ADD-4A02-9010-043E4E867A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B366C2C7-3E48-40F5-A875-6058D2E8809C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="8550" yWindow="735" windowWidth="28395" windowHeight="20040" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
   <si>
     <t>subject_id</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Hard rock shores</t>
   </si>
   <si>
-    <t>Soft rock shoes</t>
-  </si>
-  <si>
     <t>MT1.1 Rocky Shorelines</t>
   </si>
   <si>
@@ -153,23 +150,83 @@
     <t>smartline:Hard rock shores</t>
   </si>
   <si>
-    <t>smartline:Soft rock shoes</t>
-  </si>
-  <si>
     <t>smartline:Sandy shores</t>
   </si>
   <si>
     <t>smartline:Sand dune and beach ridge coasts</t>
   </si>
   <si>
-    <t>smartline: TBA</t>
+    <t>smartline:Muddy shores</t>
+  </si>
+  <si>
+    <t>Muddy shores</t>
+  </si>
+  <si>
+    <t>Coarse sediment shores</t>
+  </si>
+  <si>
+    <t>Undifferentiated sediment shores</t>
+  </si>
+  <si>
+    <t>Soft rock shores</t>
+  </si>
+  <si>
+    <t>smartline:Soft rock shores</t>
+  </si>
+  <si>
+    <t>Coral coasts</t>
+  </si>
+  <si>
+    <t>No stability classification</t>
+  </si>
+  <si>
+    <t>smartline:Coarse sediment shores</t>
+  </si>
+  <si>
+    <t>smartline:Undifferentiated sediment shores</t>
+  </si>
+  <si>
+    <t>smartline:Coral coasts</t>
+  </si>
+  <si>
+    <t>smartline:No stability classification</t>
+  </si>
+  <si>
+    <t>Rebecca Jordan</t>
+  </si>
+  <si>
+    <t>orcid:0000-0002-4048-6792</t>
+  </si>
+  <si>
+    <t>get:groups/MT1.2</t>
+  </si>
+  <si>
+    <t>MT1.2 Muddy Shorelines</t>
+  </si>
+  <si>
+    <t>skos:broadMatch</t>
+  </si>
+  <si>
+    <t>owl:Nothing</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
+  </si>
+  <si>
+    <t>smartline: https://services.ga.gov.au/gis/rest/services/Geomorphology_Smartline/MapServer</t>
+  </si>
+  <si>
+    <t>get:groups/MT1.4</t>
+  </si>
+  <si>
+    <t>MT1.4 Boulder and cobble shores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,8 +247,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F2328"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +265,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -217,13 +287,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DD23B2-5C24-4E92-A3A3-39F13C78738A}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,8 +635,8 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>41</v>
+      <c r="A3" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -608,14 +683,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
@@ -674,7 +749,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -683,10 +758,10 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -706,7 +781,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -715,10 +790,10 @@
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -738,19 +813,19 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -770,19 +845,19 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -802,19 +877,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -833,24 +908,152 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G7" s="3"/>
-      <c r="I7" s="2"/>
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="2">
+        <v>45455</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G8" s="3"/>
-      <c r="I8" s="2"/>
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="2">
+        <v>45455</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G9" s="3"/>
-      <c r="I9" s="2"/>
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="2">
+        <v>45455</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G10" s="3"/>
-      <c r="I10" s="2"/>
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="2">
+        <v>45455</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G11" s="3"/>
-      <c r="I11" s="2"/>
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="2">
+        <v>45455</v>
+      </c>
+      <c r="K11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G12" s="3"/>
@@ -930,23 +1133,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
-    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
-      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
-      <Description>63P7TJYCZHM3-28990658-16955</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -1222,7 +1408,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72d9be16-af35-44ba-8991-a3db737bf75a" xsi:nil="true"/>
+    <Notes0 xmlns="9e444dda-df07-4069-8b25-4dfb1c3da75a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">63P7TJYCZHM3-28990658-16955</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="72d9be16-af35-44ba-8991-a3db737bf75a">
+      <Url>https://csiroau.sharepoint.com/sites/CSIRO-LEAP/_layouts/15/DocIdRedir.aspx?ID=63P7TJYCZHM3-28990658-16955</Url>
+      <Description>63P7TJYCZHM3-28990658-16955</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1272,27 +1484,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
-    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1311,18 +1503,29 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
+    <ds:schemaRef ds:uri="72d9be16-af35-44ba-8991-a3db737bf75a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update to Smartline crosswalk
</commit_message>
<xml_diff>
--- a/crosswalks/Smartline-IUCNGET/Smartline-IUCNGET.xlsx
+++ b/crosswalks/Smartline-IUCNGET/Smartline-IUCNGET.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ecosystem-typology\crosswalks\Smartline-IUCNGET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/jor069_csiro_au/Documents/NEAP/ecosystem-typology_working-copies/crosswalks/Shoreline_IUCNGET/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FCA8B7-610B-42CD-8F4E-7D348952551D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{3ADDF8AC-D86F-4686-858A-73930A070093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DB35A1F-DAA8-4FD9-B90B-60CA8E5D655C}"/>
   <bookViews>
-    <workbookView xWindow="10275" yWindow="2685" windowWidth="19425" windowHeight="15345" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
-    <sheet name="header" sheetId="5" r:id="rId1"/>
-    <sheet name="SSSOM" sheetId="4" r:id="rId2"/>
+    <sheet name="Decision_rules" sheetId="6" r:id="rId1"/>
+    <sheet name="header" sheetId="5" r:id="rId2"/>
+    <sheet name="SSSOM" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>subject_id</t>
   </si>
@@ -75,12 +76,6 @@
     <t>reviewer_id</t>
   </si>
   <si>
-    <t>orcid:0009-0001-6090-9959</t>
-  </si>
-  <si>
-    <t>Craig Macfarlane</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -93,78 +88,18 @@
     <t>status:draft</t>
   </si>
   <si>
-    <t>Undifferentiated rock shores</t>
-  </si>
-  <si>
-    <t>Hard rock shores</t>
-  </si>
-  <si>
     <t>MT1.1 Rocky Shorelines</t>
   </si>
   <si>
     <t>MT1.3 Sandy Shorelines</t>
   </si>
   <si>
-    <t>Sandy shores</t>
-  </si>
-  <si>
-    <t>Sand dune and beach ridge coasts</t>
-  </si>
-  <si>
     <t>get:groups/MT1.1</t>
   </si>
   <si>
     <t>get:groups/MT1.3</t>
   </si>
   <si>
-    <t>smartline:Undifferentiated rock shores</t>
-  </si>
-  <si>
-    <t>smartline:Hard rock shores</t>
-  </si>
-  <si>
-    <t>smartline:Sandy shores</t>
-  </si>
-  <si>
-    <t>smartline:Sand dune and beach ridge coasts</t>
-  </si>
-  <si>
-    <t>smartline:Muddy shores</t>
-  </si>
-  <si>
-    <t>Muddy shores</t>
-  </si>
-  <si>
-    <t>Coarse sediment shores</t>
-  </si>
-  <si>
-    <t>Undifferentiated sediment shores</t>
-  </si>
-  <si>
-    <t>Soft rock shores</t>
-  </si>
-  <si>
-    <t>smartline:Soft rock shores</t>
-  </si>
-  <si>
-    <t>Coral coasts</t>
-  </si>
-  <si>
-    <t>No stability classification</t>
-  </si>
-  <si>
-    <t>smartline:Coarse sediment shores</t>
-  </si>
-  <si>
-    <t>smartline:Undifferentiated sediment shores</t>
-  </si>
-  <si>
-    <t>smartline:Coral coasts</t>
-  </si>
-  <si>
-    <t>smartline:No stability classification</t>
-  </si>
-  <si>
     <t>Rebecca Jordan</t>
   </si>
   <si>
@@ -177,50 +112,83 @@
     <t>MT1.2 Muddy Shorelines</t>
   </si>
   <si>
-    <t>skos:broadMatch</t>
-  </si>
-  <si>
-    <t>owl:Nothing</t>
-  </si>
-  <si>
-    <t>Unclassified</t>
-  </si>
-  <si>
     <t>get:groups/MT1.4</t>
   </si>
   <si>
     <t>MT1.4 Boulder and cobble shores</t>
   </si>
   <si>
-    <t>orcid: https://orcid.org/</t>
-  </si>
-  <si>
-    <t>sssom: https://w3id.org/sssom/</t>
-  </si>
-  <si>
-    <t>semapv: https://w3id.org/semapv/vocab/</t>
-  </si>
-  <si>
-    <t>crosswalk: https://w3id.org/env/neap/crosswalk/</t>
-  </si>
-  <si>
-    <t>status: https://w3id.org/env/neap/status/</t>
-  </si>
-  <si>
-    <t>get: https://global-ecosystems.org/explore/</t>
-  </si>
-  <si>
-    <t>smartline: https://w3id.org/env/neap/smartline/</t>
-  </si>
-  <si>
-    <t>map: http://w3id.org/env/neap/smartline-get/</t>
+    <t xml:space="preserve">creator_id: </t>
+  </si>
+  <si>
+    <t>curie_map:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   orcid: https://orcid.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   sssom: https://w3id.org/sssom/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   semapv: https://w3id.org/semapv/vocab/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   status: https://w3id.org/env/neap/status/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   get: https://global-ecosystems.org/explore/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   map: http://w3id.org/env/neap/smartline-get/</t>
+  </si>
+  <si>
+    <t>mapping_set_id:</t>
+  </si>
+  <si>
+    <t>license:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   skos: http://www.w3.org/2004/02/skos/core#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   shoreline: derived data (based on GA Smartline)</t>
+  </si>
+  <si>
+    <t>shoreline:MT1.1_Rocky_Shorelines</t>
+  </si>
+  <si>
+    <t>shoreline:MT1.2_Muddy_Shorelines</t>
+  </si>
+  <si>
+    <t>shoreline:MT1.3_Sandy_Shorelines</t>
+  </si>
+  <si>
+    <t>shoreline:MT1.4_Boulder_and_cobble_shores</t>
+  </si>
+  <si>
+    <t>else if:  "HARDROCK_V" is not NA =&gt; MT1.1 Rocky Shorelines</t>
+  </si>
+  <si>
+    <t>else if: "MUDDY_V" is not NA =&gt; MT1.2 Muddy Shorelines</t>
+  </si>
+  <si>
+    <t>else if: "COARSED_V" is not NA =&gt; MT1.4 Boulder and cobble shores</t>
+  </si>
+  <si>
+    <t>if: "SANDY_V" is not NA =&gt; MT1.3 Sandy Shorelines</t>
+  </si>
+  <si>
+    <t>Priority order from lowest to highest is 'COARSED_V' -&gt; 'MUDDY_V' -&gt; 'ROCKY_V' -&gt; 'SANDY_V'</t>
+  </si>
+  <si>
+    <t>such that a shoreline segment is only classified as 'boulder and cobble' if the segment is 'not identified as' muddy or rocky or sandy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,13 +208,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1F2328"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -292,9 +253,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -302,12 +263,9 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,11 +580,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99ACCAF7-2FDD-40DD-A5D1-7768B48E3A53}">
+  <dimension ref="A2:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DD23B2-5C24-4E92-A3A3-39F13C78738A}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,43 +643,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>51</v>
+      <c r="A1" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>52</v>
+      <c r="A2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>54</v>
+      <c r="A4" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>55</v>
+      <c r="A5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>56</v>
+      <c r="A6" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>57</v>
+      <c r="A7" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>58</v>
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -679,17 +707,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -728,7 +756,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -737,7 +765,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
@@ -749,311 +777,155 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I2" s="2">
-        <v>45422</v>
+        <v>45474</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I3" s="2">
-        <v>45422</v>
+        <v>45474</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I4" s="2">
-        <v>45422</v>
+        <v>45474</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I5" s="2">
-        <v>45422</v>
+        <v>45474</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="2">
-        <v>45422</v>
-      </c>
-      <c r="K6" t="s">
-        <v>17</v>
-      </c>
+      <c r="G6" s="3"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="2">
-        <v>45455</v>
-      </c>
-      <c r="K7" t="s">
-        <v>17</v>
-      </c>
+      <c r="G7" s="3"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="2">
-        <v>45455</v>
-      </c>
-      <c r="K8" t="s">
-        <v>17</v>
-      </c>
+      <c r="G8" s="3"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="2">
-        <v>45455</v>
-      </c>
-      <c r="K9" t="s">
-        <v>17</v>
-      </c>
+      <c r="G9" s="3"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="2">
-        <v>45455</v>
-      </c>
-      <c r="K10" t="s">
-        <v>17</v>
-      </c>
+      <c r="G10" s="3"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="2">
-        <v>45455</v>
-      </c>
-      <c r="K11" t="s">
-        <v>17</v>
-      </c>
+      <c r="G11" s="3"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G12" s="3"/>
@@ -1085,46 +957,6 @@
     </row>
     <row r="19" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G19" s="3"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G20" s="3"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G21" s="3"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G22" s="3"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G23" s="3"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G24" s="3"/>
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G25" s="3"/>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G26" s="3"/>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G27" s="3"/>
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G28" s="3"/>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1150,6 +982,65 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -1425,65 +1316,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
   <ds:schemaRefs>
@@ -1496,6 +1328,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1512,20 +1360,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>